<commit_message>
Modifica al funzionamento del sorting per l'euristico (priorità cliente con segno corretto, due date forte per commesse "esterne"); sistemati gli euristici per commesse "esterne" (zona zero)
</commit_message>
<xml_diff>
--- a/PS-VRP/INPUT_TEST/VEICOLI9.xlsx
+++ b/PS-VRP/INPUT_TEST/VEICOLI9.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wikipedis\Documents\GitHub\progettoIS\PS-VRP\INPUT_TEST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frenc\Documents\GitHub\progettoIS\PS-VRP\INPUT_TEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F1E0E4-325B-4021-9E65-3923E2D3951E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400916BC-3894-4682-9FDA-D7D184745F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{BA5BC94F-5D6C-4899-9888-A4EA67F19BD8}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="21600" windowHeight="11295" xr2:uid="{BA5BC94F-5D6C-4899-9888-A4EA67F19BD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -440,7 +440,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A11" sqref="A11:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Cambiamenti al check e al filtro commesse
</commit_message>
<xml_diff>
--- a/PS-VRP/INPUT_TEST/VEICOLI9.xlsx
+++ b/PS-VRP/INPUT_TEST/VEICOLI9.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frenc\Documents\GitHub\progettoIS\PS-VRP\INPUT_TEST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wikipedis\Documents\GitHub\progettoIS\PS-VRP\INPUT_TEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400916BC-3894-4682-9FDA-D7D184745F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B41B6C-3082-4C48-8B7C-1D4F64D12FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="21600" windowHeight="11295" xr2:uid="{BA5BC94F-5D6C-4899-9888-A4EA67F19BD8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BA5BC94F-5D6C-4899-9888-A4EA67F19BD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -440,7 +440,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:E11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,7 +510,7 @@
         <v>45660</v>
       </c>
       <c r="C4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1">
         <v>6000</v>
@@ -527,7 +527,7 @@
         <v>45661</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1">
         <v>10000</v>
@@ -544,7 +544,7 @@
         <v>45662</v>
       </c>
       <c r="C6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1">
         <v>8000</v>
@@ -561,7 +561,7 @@
         <v>45663</v>
       </c>
       <c r="C7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="1">
         <v>10000</v>
@@ -578,7 +578,7 @@
         <v>45664</v>
       </c>
       <c r="C8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="1">
         <v>10000</v>
@@ -595,7 +595,7 @@
         <v>45665</v>
       </c>
       <c r="C9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="1">
         <v>10000</v>
@@ -612,7 +612,7 @@
         <v>45666</v>
       </c>
       <c r="C10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="1">
         <v>10000</v>

</xml_diff>

<commit_message>
Implementati i check anche per le altre ricerche locali
</commit_message>
<xml_diff>
--- a/PS-VRP/INPUT_TEST/VEICOLI9.xlsx
+++ b/PS-VRP/INPUT_TEST/VEICOLI9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wikipedis\Documents\GitHub\progettoIS\PS-VRP\INPUT_TEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B41B6C-3082-4C48-8B7C-1D4F64D12FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B746C5B-5D95-42CA-BDAB-03A34C42BF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BA5BC94F-5D6C-4899-9888-A4EA67F19BD8}"/>
   </bookViews>
@@ -440,7 +440,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,7 +510,7 @@
         <v>45660</v>
       </c>
       <c r="C4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1">
         <v>6000</v>
@@ -527,7 +527,7 @@
         <v>45661</v>
       </c>
       <c r="C5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
         <v>10000</v>
@@ -544,7 +544,7 @@
         <v>45662</v>
       </c>
       <c r="C6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1">
         <v>8000</v>
@@ -561,7 +561,7 @@
         <v>45663</v>
       </c>
       <c r="C7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1">
         <v>10000</v>
@@ -578,7 +578,7 @@
         <v>45664</v>
       </c>
       <c r="C8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1">
         <v>10000</v>
@@ -595,7 +595,7 @@
         <v>45665</v>
       </c>
       <c r="C9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="1">
         <v>10000</v>
@@ -612,7 +612,7 @@
         <v>45666</v>
       </c>
       <c r="C10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="1">
         <v>10000</v>

</xml_diff>